<commit_message>
Nuevo formulario funcional en entradas y salidas
</commit_message>
<xml_diff>
--- a/Prueba 1.xlsx
+++ b/Prueba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\TFG\app-gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13BCA83-E404-4501-8248-7642ED357C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D871D75-D474-4368-929A-2A28B07C4EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-5364" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20736" yWindow="3852" windowWidth="12960" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TFG" sheetId="1" r:id="rId1"/>
@@ -372,7 +372,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B10" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -420,9 +420,7 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2">
-        <v>1122334455</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="3">
         <v>8354456</v>
       </c>
@@ -447,9 +445,7 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
-        <v>9876543210</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="1">
         <v>7545678</v>
       </c>
@@ -474,9 +470,7 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
-        <v>5678901234</v>
-      </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="1">
         <v>1234567</v>
       </c>
@@ -603,9 +597,7 @@
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>9876543210</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="1">
         <v>1122334</v>
       </c>
@@ -630,9 +622,7 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <v>5678901234</v>
-      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="1">
         <v>4433221</v>
       </c>

</xml_diff>

<commit_message>
corrección de fallos tras reunión en Delim
</commit_message>
<xml_diff>
--- a/Prueba 1.xlsx
+++ b/Prueba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\TFG\app-gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4195E7B9-253B-4E3D-9FBE-C2B2B2EF7B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF45774E-DAA7-4837-9FFB-5F49E0D5BC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-5028" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TFG" sheetId="1" r:id="rId1"/>
@@ -372,22 +372,22 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" customWidth="1"/>
-    <col min="8" max="9" width="5.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="9" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -416,7 +416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -441,7 +441,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -466,7 +466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -491,7 +491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -518,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -543,7 +543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -568,7 +568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -593,7 +593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -618,7 +618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -643,7 +643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -654,7 +654,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -665,7 +665,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -676,7 +676,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -687,7 +687,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -698,7 +698,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
@@ -709,7 +709,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
@@ -720,7 +720,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>

</xml_diff>

<commit_message>
Estados funcionando de forma local al menos
</commit_message>
<xml_diff>
--- a/Prueba 1.xlsx
+++ b/Prueba 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\TFG\app-gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF45774E-DAA7-4837-9FFB-5F49E0D5BC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E39C669-7ECE-4E83-A8F7-7410028D214B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TFG" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>dcs</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t>REF</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>OPCC</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
+  <si>
+    <t>TRUCK</t>
+  </si>
+  <si>
+    <t>INVENT</t>
   </si>
 </sst>
 </file>
@@ -369,25 +384,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="9" width="5.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" customWidth="1"/>
+    <col min="8" max="9" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -415,8 +430,11 @@
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -440,8 +458,11 @@
       <c r="I2" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -465,8 +486,11 @@
       <c r="I3" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -490,8 +514,11 @@
       <c r="I4" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -517,8 +544,11 @@
       <c r="I5" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,8 +572,11 @@
       <c r="I6" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -567,8 +600,11 @@
       <c r="I7" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -592,8 +628,11 @@
       <c r="I8" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -617,8 +656,11 @@
       <c r="I9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,8 +684,11 @@
       <c r="I10" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
@@ -654,7 +699,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
@@ -665,7 +710,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
@@ -676,7 +721,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -687,7 +732,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
@@ -698,7 +743,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
@@ -709,7 +754,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
@@ -720,7 +765,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>

</xml_diff>